<commit_message>
Checking that all is working ok
</commit_message>
<xml_diff>
--- a/Docs/Tarea programada 1 - documentación/Tarea programada 1 - Pruebas y resultados.xlsx
+++ b/Docs/Tarea programada 1 - documentación/Tarea programada 1 - Pruebas y resultados.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Dropbox\IC-4302 Bases de datos II\Tarea programada 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Google Drive\TEC\BD II\Works_Projects\Proyecto 1\Docs\Tarea programada 1 - documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE407F2-BC06-4F91-B629-5CB2F2271B4D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5880" tabRatio="355" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19176" windowHeight="9048" tabRatio="527" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="2" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="157">
   <si>
     <t>Betina Guardado Samaniego</t>
   </si>
@@ -481,9 +482,6 @@
     <t>Admin.</t>
   </si>
   <si>
-    <t>SÍ / NO</t>
-  </si>
-  <si>
     <t>crear participante</t>
   </si>
   <si>
@@ -560,9 +558,6 @@
   </si>
   <si>
     <t>Listar subastas (Estampillas &gt; Latinoamerica) - debe aparecer Serie árboles de Costa Rica</t>
-  </si>
-  <si>
-    <t>¿OK?</t>
   </si>
   <si>
     <t>Al finalizar usar consultas para:
@@ -596,11 +591,20 @@
       <t xml:space="preserve"> si las acciones fueron ejecutadas correctamente (OK) , o si hubo inconvenientes.</t>
     </r>
   </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>SÍ</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -643,12 +647,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB9B9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="16">
@@ -837,7 +859,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1050,6 +1072,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1059,34 +1093,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFB9B9"/>
+      <color rgb="FFFF6D6D"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1360,26 +1406,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.54296875" customWidth="1"/>
-    <col min="2" max="2" width="8.08984375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.54296875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.36328125" customWidth="1"/>
-    <col min="8" max="8" width="12.6328125" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="14" t="s">
         <v>65</v>
       </c>
@@ -1405,7 +1451,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="2:9" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
         <v>63</v>
       </c>
@@ -1429,7 +1475,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
         <v>63</v>
       </c>
@@ -1453,7 +1499,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="15" t="s">
         <v>63</v>
       </c>
@@ -1477,7 +1523,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
       <c r="D6" s="12"/>
@@ -1487,7 +1533,7 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="15" t="s">
         <v>64</v>
       </c>
@@ -1513,7 +1559,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
         <v>64</v>
       </c>
@@ -1537,7 +1583,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="s">
         <v>64</v>
       </c>
@@ -1561,7 +1607,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
         <v>64</v>
       </c>
@@ -1585,7 +1631,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
         <v>64</v>
       </c>
@@ -1609,7 +1655,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
         <v>64</v>
       </c>
@@ -1633,7 +1679,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
         <v>64</v>
       </c>
@@ -1657,7 +1703,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
       <c r="E14" s="7"/>
@@ -1666,7 +1712,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C15" s="2"/>
       <c r="D15" s="3"/>
       <c r="E15" s="7"/>
@@ -1675,28 +1721,28 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="5"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="5"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="5"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="5"/>
@@ -1705,16 +1751,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1"/>
-    <hyperlink ref="G12" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G13" r:id="rId4"/>
-    <hyperlink ref="G5" r:id="rId5"/>
-    <hyperlink ref="G7" r:id="rId6"/>
-    <hyperlink ref="G8" r:id="rId7"/>
-    <hyperlink ref="G9" r:id="rId8"/>
-    <hyperlink ref="G10" r:id="rId9"/>
-    <hyperlink ref="G11" r:id="rId10"/>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G13" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>
@@ -1722,27 +1768,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.6328125" customWidth="1"/>
-    <col min="2" max="2" width="4.81640625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="4.77734375" style="8" customWidth="1"/>
     <col min="3" max="3" width="66" customWidth="1"/>
-    <col min="4" max="4" width="1.6328125" customWidth="1"/>
-    <col min="5" max="5" width="10.90625" style="1"/>
-    <col min="6" max="6" width="1.6328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.90625" style="1"/>
-    <col min="8" max="8" width="1.6328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="39.54296875" customWidth="1"/>
+    <col min="4" max="4" width="1.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" style="1"/>
+    <col min="6" max="6" width="1.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" style="1"/>
+    <col min="8" max="8" width="1.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="39.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="73" t="s">
         <v>77</v>
       </c>
@@ -1750,16 +1796,16 @@
       <c r="D2" s="73"/>
       <c r="E2" s="73"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C3" s="74" t="s">
         <v>76</v>
       </c>
       <c r="D3" s="74"/>
       <c r="E3" s="74"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C4" s="29" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D4" s="29"/>
       <c r="E4" s="7"/>
@@ -1767,7 +1813,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="75" t="s">
         <v>118</v>
       </c>
@@ -1777,11 +1823,11 @@
       <c r="G5" s="75"/>
       <c r="H5" s="28"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="11"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="76" t="s">
         <v>117</v>
       </c>
@@ -1792,11 +1838,11 @@
       <c r="G7" s="76"/>
       <c r="H7" s="30"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="11"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="2:9" s="6" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:9" s="6" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="33" t="s">
         <v>74</v>
       </c>
@@ -1822,7 +1868,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="2:9" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:9" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="14">
         <v>0</v>
       </c>
@@ -1835,7 +1881,7 @@
       <c r="H10" s="1"/>
       <c r="I10"/>
     </row>
-    <row r="11" spans="2:9" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:9" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="E11" s="1"/>
@@ -1843,7 +1889,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="10">
         <v>1</v>
       </c>
@@ -1851,13 +1897,13 @@
         <v>46</v>
       </c>
       <c r="E12" s="67" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G12" s="67" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="10"/>
       <c r="C13" s="23" t="s">
         <v>45</v>
@@ -1865,530 +1911,581 @@
       <c r="E13" s="68"/>
       <c r="G13" s="68"/>
     </row>
-    <row r="14" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C14" s="25" t="s">
         <v>47</v>
       </c>
       <c r="E14" s="69"/>
       <c r="G14" s="69"/>
     </row>
-    <row r="15" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="8">
         <v>3</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="E16" s="67"/>
-      <c r="G16" s="67"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="E16" s="67" t="s">
+        <v>154</v>
+      </c>
+      <c r="G16" s="67" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C17" s="24" t="s">
         <v>100</v>
       </c>
       <c r="E17" s="68"/>
       <c r="G17" s="68"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C18" s="24" t="s">
         <v>101</v>
       </c>
       <c r="E18" s="68"/>
       <c r="G18" s="68"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C19" s="24" t="s">
         <v>102</v>
       </c>
       <c r="E19" s="68"/>
       <c r="G19" s="68"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C20" s="24" t="s">
         <v>81</v>
       </c>
       <c r="E20" s="68"/>
       <c r="G20" s="68"/>
     </row>
-    <row r="21" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C21" s="25" t="s">
         <v>47</v>
       </c>
       <c r="E21" s="69"/>
       <c r="G21" s="69"/>
     </row>
-    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="8">
         <v>4</v>
       </c>
       <c r="C23" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="67"/>
-      <c r="G23" s="67"/>
-      <c r="I23" s="70" t="s">
+      <c r="E23" s="67" t="s">
+        <v>154</v>
+      </c>
+      <c r="G23" s="67" t="s">
+        <v>154</v>
+      </c>
+      <c r="I23" s="92" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C24" s="23" t="s">
         <v>82</v>
       </c>
       <c r="E24" s="68"/>
       <c r="G24" s="68"/>
-      <c r="I24" s="71"/>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I24" s="93"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C25" s="24" t="s">
         <v>103</v>
       </c>
       <c r="E25" s="68"/>
       <c r="G25" s="68"/>
-      <c r="I25" s="71"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I25" s="93"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C26" s="24" t="s">
         <v>104</v>
       </c>
       <c r="E26" s="68"/>
       <c r="G26" s="68"/>
-      <c r="I26" s="71"/>
-    </row>
-    <row r="27" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I26" s="93"/>
+    </row>
+    <row r="27" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C27" s="25" t="s">
         <v>47</v>
       </c>
       <c r="E27" s="69"/>
       <c r="G27" s="69"/>
-      <c r="I27" s="72"/>
-    </row>
-    <row r="28" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I27" s="94"/>
+    </row>
+    <row r="28" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="8">
         <v>5</v>
       </c>
       <c r="C29" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="E29" s="67"/>
-      <c r="G29" s="67"/>
-    </row>
-    <row r="30" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="E29" s="67" t="s">
+        <v>154</v>
+      </c>
+      <c r="G29" s="67" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C30" s="24" t="s">
         <v>54</v>
       </c>
       <c r="E30" s="68"/>
       <c r="G30" s="68"/>
     </row>
-    <row r="31" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C31" s="25" t="s">
         <v>47</v>
       </c>
       <c r="E31" s="69"/>
       <c r="G31" s="69"/>
     </row>
-    <row r="32" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="8">
         <v>6</v>
       </c>
       <c r="C33" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="E33" s="67"/>
-      <c r="G33" s="67"/>
-    </row>
-    <row r="34" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="E33" s="67" t="s">
+        <v>154</v>
+      </c>
+      <c r="G33" s="67" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C34" s="24" t="s">
         <v>58</v>
       </c>
       <c r="E34" s="68"/>
       <c r="G34" s="68"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C35" s="24" t="s">
         <v>49</v>
       </c>
       <c r="E35" s="68"/>
       <c r="G35" s="68"/>
     </row>
-    <row r="36" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C36" s="25" t="s">
         <v>47</v>
       </c>
       <c r="E36" s="69"/>
       <c r="G36" s="69"/>
     </row>
-    <row r="37" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C37" s="2"/>
     </row>
-    <row r="38" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="8">
         <v>7</v>
       </c>
       <c r="C38" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="E38" s="67"/>
-      <c r="G38" s="67"/>
-      <c r="I38" s="70" t="s">
+      <c r="E38" s="67" t="s">
+        <v>154</v>
+      </c>
+      <c r="G38" s="67" t="s">
+        <v>154</v>
+      </c>
+      <c r="I38" s="92" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C39" s="24" t="s">
         <v>58</v>
       </c>
       <c r="E39" s="68"/>
       <c r="G39" s="68"/>
-      <c r="I39" s="71"/>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="C40" s="24" t="s">
+      <c r="I39" s="93"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C40" s="91" t="s">
         <v>50</v>
       </c>
       <c r="E40" s="68"/>
       <c r="G40" s="68"/>
-      <c r="I40" s="71"/>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I40" s="93"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C41" s="24" t="s">
         <v>51</v>
       </c>
       <c r="E41" s="68"/>
       <c r="G41" s="68"/>
-      <c r="I41" s="71"/>
-    </row>
-    <row r="42" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="I41" s="93"/>
+    </row>
+    <row r="42" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C42" s="24" t="s">
         <v>59</v>
       </c>
       <c r="E42" s="68"/>
       <c r="G42" s="68"/>
-      <c r="I42" s="71"/>
-    </row>
-    <row r="43" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="I42" s="93"/>
+    </row>
+    <row r="43" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C43" s="24" t="s">
         <v>52</v>
       </c>
       <c r="E43" s="68"/>
       <c r="G43" s="68"/>
-      <c r="I43" s="71"/>
-    </row>
-    <row r="44" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="I43" s="93"/>
+    </row>
+    <row r="44" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C44" s="24" t="s">
         <v>60</v>
       </c>
       <c r="E44" s="68"/>
       <c r="G44" s="68"/>
-      <c r="I44" s="71"/>
-    </row>
-    <row r="45" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I44" s="93"/>
+    </row>
+    <row r="45" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C45" s="25" t="s">
         <v>47</v>
       </c>
       <c r="E45" s="69"/>
       <c r="G45" s="69"/>
-      <c r="I45" s="72"/>
-    </row>
-    <row r="46" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I45" s="94"/>
+    </row>
+    <row r="46" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C46" s="2"/>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B47" s="8">
         <v>8</v>
       </c>
       <c r="C47" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="E47" s="67"/>
-      <c r="G47" s="67"/>
-    </row>
-    <row r="48" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="E47" s="67" t="s">
+        <v>154</v>
+      </c>
+      <c r="G47" s="67" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C48" s="24" t="s">
         <v>60</v>
       </c>
       <c r="E48" s="68"/>
       <c r="G48" s="68"/>
     </row>
-    <row r="49" spans="2:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="C49" s="24" t="s">
+    <row r="49" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C49" s="90" t="s">
         <v>53</v>
       </c>
       <c r="E49" s="68"/>
       <c r="G49" s="68"/>
     </row>
-    <row r="50" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C50" s="25" t="s">
         <v>47</v>
       </c>
       <c r="E50" s="69"/>
       <c r="G50" s="69"/>
     </row>
-    <row r="51" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C51" s="2"/>
     </row>
-    <row r="52" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="8">
         <v>9</v>
       </c>
       <c r="C52" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="E52" s="67"/>
-      <c r="G52" s="67"/>
-    </row>
-    <row r="53" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="E52" s="67" t="s">
+        <v>154</v>
+      </c>
+      <c r="G52" s="67" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C53" s="24" t="s">
         <v>80</v>
       </c>
       <c r="E53" s="68"/>
       <c r="G53" s="68"/>
     </row>
-    <row r="54" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C54" s="25" t="s">
         <v>47</v>
       </c>
       <c r="E54" s="69"/>
       <c r="G54" s="69"/>
     </row>
-    <row r="55" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C55" s="2"/>
     </row>
-    <row r="56" spans="2:9" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:9" s="4" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="14">
         <v>11</v>
       </c>
       <c r="C56" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="E56" s="67"/>
+      <c r="E56" s="67" t="s">
+        <v>154</v>
+      </c>
       <c r="F56" s="7"/>
-      <c r="G56" s="67"/>
+      <c r="G56" s="67" t="s">
+        <v>154</v>
+      </c>
       <c r="H56" s="7"/>
       <c r="I56"/>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C57" s="24" t="s">
         <v>56</v>
       </c>
       <c r="E57" s="68"/>
       <c r="G57" s="68"/>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C58" s="24" t="s">
         <v>57</v>
       </c>
       <c r="E58" s="68"/>
       <c r="G58" s="68"/>
     </row>
-    <row r="59" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C59" s="25" t="s">
         <v>47</v>
       </c>
       <c r="E59" s="69"/>
       <c r="G59" s="69"/>
     </row>
-    <row r="60" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="8">
         <v>12</v>
       </c>
       <c r="C61" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="E61" s="67"/>
-      <c r="G61" s="67"/>
-      <c r="I61" s="70" t="s">
+      <c r="E61" s="67" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="G61" s="67" t="s">
+        <v>154</v>
+      </c>
+      <c r="I61" s="92" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C62" s="24" t="s">
         <v>84</v>
       </c>
       <c r="E62" s="68"/>
       <c r="G62" s="68"/>
-      <c r="I62" s="71"/>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I62" s="93"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C63" s="24" t="s">
         <v>85</v>
       </c>
       <c r="E63" s="68"/>
       <c r="G63" s="68"/>
-      <c r="I63" s="71"/>
-    </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I63" s="93"/>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C64" s="24" t="s">
         <v>83</v>
       </c>
       <c r="E64" s="68"/>
       <c r="G64" s="68"/>
-      <c r="I64" s="71"/>
-    </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I64" s="93"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C65" s="24" t="s">
         <v>55</v>
       </c>
       <c r="E65" s="68"/>
       <c r="G65" s="68"/>
-      <c r="I65" s="71"/>
-    </row>
-    <row r="66" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I65" s="93"/>
+    </row>
+    <row r="66" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C66" s="25" t="s">
         <v>47</v>
       </c>
       <c r="E66" s="69"/>
       <c r="G66" s="69"/>
-      <c r="I66" s="72"/>
-    </row>
-    <row r="67" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I66" s="94"/>
+    </row>
+    <row r="67" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C67" s="2"/>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B68" s="8">
         <v>13</v>
       </c>
       <c r="C68" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="E68" s="67"/>
-      <c r="G68" s="67"/>
-    </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="E68" s="67" t="s">
+        <v>154</v>
+      </c>
+      <c r="G68" s="67" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C69" s="24" t="s">
         <v>61</v>
       </c>
       <c r="E69" s="68"/>
       <c r="G69" s="68"/>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C70" s="24" t="s">
         <v>62</v>
       </c>
       <c r="E70" s="68"/>
       <c r="G70" s="68"/>
     </row>
-    <row r="71" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C71" s="25" t="s">
         <v>47</v>
       </c>
       <c r="E71" s="69"/>
       <c r="G71" s="69"/>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C72" s="39"/>
       <c r="E72" s="40"/>
       <c r="G72" s="40"/>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C73" s="39"/>
       <c r="E73" s="40"/>
       <c r="G73" s="40"/>
     </row>
-    <row r="74" spans="2:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G74" s="31" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="75" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E74" s="31" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="8">
         <v>14</v>
       </c>
       <c r="C75" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="G75" s="67" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="76" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="E75" s="67" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C76" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="G76" s="68"/>
-    </row>
-    <row r="77" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>148</v>
+      </c>
+      <c r="E76" s="68"/>
+    </row>
+    <row r="77" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C77" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="G77" s="69"/>
-    </row>
-    <row r="78" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="E77" s="69"/>
+    </row>
+    <row r="78" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B79" s="8">
         <v>15</v>
       </c>
       <c r="C79" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="G79" s="67"/>
+      <c r="E79" s="67" t="s">
+        <v>154</v>
+      </c>
       <c r="I79" s="70" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="80" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C80" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="G80" s="68"/>
+        <v>151</v>
+      </c>
+      <c r="E80" s="68"/>
       <c r="I80" s="71"/>
     </row>
-    <row r="81" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C81" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="E81" s="68"/>
+      <c r="I81" s="71"/>
+    </row>
+    <row r="82" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C82" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="G81" s="68"/>
-      <c r="I81" s="71"/>
-    </row>
-    <row r="82" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C82" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="G82" s="68"/>
+      <c r="E82" s="68"/>
       <c r="I82" s="71"/>
     </row>
-    <row r="83" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C83" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="G83" s="68"/>
+      <c r="E83" s="68"/>
       <c r="I83" s="71"/>
     </row>
-    <row r="84" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C84" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="G84" s="68"/>
+      <c r="E84" s="68"/>
       <c r="I84" s="71"/>
     </row>
-    <row r="85" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="85" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C85" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="G85" s="69"/>
+      <c r="E85" s="69"/>
       <c r="I85" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="E16:E21"/>
-    <mergeCell ref="G16:G21"/>
-    <mergeCell ref="G52:G54"/>
+    <mergeCell ref="E79:E85"/>
+    <mergeCell ref="I79:I85"/>
+    <mergeCell ref="E75:E77"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="I38:I45"/>
+    <mergeCell ref="I61:I66"/>
+    <mergeCell ref="I23:I27"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="E56:E59"/>
+    <mergeCell ref="E61:E66"/>
+    <mergeCell ref="E68:E71"/>
     <mergeCell ref="G56:G59"/>
     <mergeCell ref="G61:G66"/>
     <mergeCell ref="G68:G71"/>
@@ -2402,20 +2499,11 @@
     <mergeCell ref="G33:G36"/>
     <mergeCell ref="G38:G45"/>
     <mergeCell ref="G47:G50"/>
-    <mergeCell ref="G79:G85"/>
-    <mergeCell ref="I79:I85"/>
-    <mergeCell ref="G75:G77"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="I38:I45"/>
-    <mergeCell ref="I61:I66"/>
-    <mergeCell ref="I23:I27"/>
-    <mergeCell ref="E52:E54"/>
-    <mergeCell ref="E56:E59"/>
-    <mergeCell ref="E61:E66"/>
-    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="E16:E21"/>
+    <mergeCell ref="G16:G21"/>
+    <mergeCell ref="G52:G54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2423,45 +2511,45 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:N28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.54296875" style="41" customWidth="1"/>
-    <col min="2" max="2" width="3.54296875" style="41" customWidth="1"/>
-    <col min="3" max="3" width="51.81640625" style="41" customWidth="1"/>
-    <col min="4" max="4" width="14.81640625" style="43" customWidth="1"/>
-    <col min="5" max="5" width="3.453125" style="41" customWidth="1"/>
-    <col min="6" max="8" width="11.54296875" style="41" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" style="43"/>
-    <col min="10" max="16384" width="10.90625" style="41"/>
+    <col min="1" max="1" width="4.5546875" style="41" customWidth="1"/>
+    <col min="2" max="2" width="3.5546875" style="41" customWidth="1"/>
+    <col min="3" max="3" width="51.77734375" style="41" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" style="43" customWidth="1"/>
+    <col min="5" max="5" width="3.44140625" style="41" customWidth="1"/>
+    <col min="6" max="8" width="11.5546875" style="41" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" style="43"/>
+    <col min="10" max="16384" width="10.88671875" style="41"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C2" s="42" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="42"/>
       <c r="C4" s="42"/>
       <c r="D4" s="44"/>
       <c r="E4" s="42"/>
-      <c r="F4" s="83" t="s">
+      <c r="F4" s="88" t="s">
         <v>121</v>
       </c>
-      <c r="G4" s="84"/>
+      <c r="G4" s="89"/>
       <c r="H4" s="45" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:14" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="46" t="s">
         <v>123</v>
       </c>
@@ -2473,46 +2561,46 @@
         <v>125</v>
       </c>
       <c r="G5" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="H5" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="J5" s="80" t="s">
+        <v>146</v>
+      </c>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="80"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C6" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="H5" s="48" t="s">
-        <v>140</v>
-      </c>
-      <c r="J5" s="89" t="s">
-        <v>147</v>
-      </c>
-      <c r="K5" s="89"/>
-      <c r="L5" s="89"/>
-      <c r="M5" s="89"/>
-      <c r="N5" s="89"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="C6" s="49" t="s">
-        <v>141</v>
-      </c>
       <c r="D6" s="50" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="F6" s="51" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="G6" s="52"/>
       <c r="H6" s="50"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="87"/>
-      <c r="L6" s="87"/>
-      <c r="M6" s="87"/>
-      <c r="N6" s="88"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="J6" s="81"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
+      <c r="N6" s="83"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C7" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="F7" s="53" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="G7" s="54"/>
       <c r="H7" s="35"/>
@@ -2522,15 +2610,15 @@
       <c r="M7" s="78"/>
       <c r="N7" s="79"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C8" s="34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="F8" s="53" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="G8" s="54"/>
       <c r="H8" s="35"/>
@@ -2540,10 +2628,10 @@
       <c r="M8" s="78"/>
       <c r="N8" s="79"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C9" s="34"/>
       <c r="D9" s="35"/>
-      <c r="F9" s="55"/>
+      <c r="F9" s="53"/>
       <c r="G9" s="56"/>
       <c r="H9" s="57"/>
       <c r="J9" s="77"/>
@@ -2552,15 +2640,15 @@
       <c r="M9" s="78"/>
       <c r="N9" s="79"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C10" s="34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="F10" s="53" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="G10" s="54"/>
       <c r="H10" s="35"/>
@@ -2570,15 +2658,15 @@
       <c r="M10" s="78"/>
       <c r="N10" s="79"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C11" s="34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="F11" s="53" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="G11" s="54"/>
       <c r="H11" s="35"/>
@@ -2588,7 +2676,7 @@
       <c r="M11" s="78"/>
       <c r="N11" s="79"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C12" s="34"/>
       <c r="D12" s="35"/>
       <c r="F12" s="55"/>
@@ -2600,19 +2688,21 @@
       <c r="M12" s="78"/>
       <c r="N12" s="79"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C13" s="34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="F13" s="53"/>
+        <v>155</v>
+      </c>
+      <c r="F13" s="53" t="s">
+        <v>155</v>
+      </c>
       <c r="G13" s="54" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="H13" s="35" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="J13" s="77"/>
       <c r="K13" s="78"/>
@@ -2620,19 +2710,21 @@
       <c r="M13" s="78"/>
       <c r="N13" s="79"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C14" s="34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="F14" s="53"/>
+        <v>155</v>
+      </c>
+      <c r="F14" s="53" t="s">
+        <v>155</v>
+      </c>
       <c r="G14" s="54" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="H14" s="35" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="J14" s="77"/>
       <c r="K14" s="78"/>
@@ -2640,7 +2732,7 @@
       <c r="M14" s="78"/>
       <c r="N14" s="79"/>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C15" s="34"/>
       <c r="D15" s="35"/>
       <c r="F15" s="55"/>
@@ -2652,21 +2744,21 @@
       <c r="M15" s="78"/>
       <c r="N15" s="79"/>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C16" s="34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="F16" s="53" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="G16" s="54" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="H16" s="35" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="J16" s="77"/>
       <c r="K16" s="78"/>
@@ -2674,21 +2766,21 @@
       <c r="M16" s="78"/>
       <c r="N16" s="79"/>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C17" s="34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="F17" s="53" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="G17" s="54" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="H17" s="35" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="J17" s="77"/>
       <c r="K17" s="78"/>
@@ -2696,21 +2788,21 @@
       <c r="M17" s="78"/>
       <c r="N17" s="79"/>
     </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C18" s="34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="F18" s="53" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="G18" s="54" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="H18" s="35" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="J18" s="77"/>
       <c r="K18" s="78"/>
@@ -2718,115 +2810,132 @@
       <c r="M18" s="78"/>
       <c r="N18" s="79"/>
     </row>
-    <row r="19" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C19" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="F19" s="58" t="s">
+        <v>155</v>
+      </c>
+      <c r="G19" s="59" t="s">
+        <v>155</v>
+      </c>
+      <c r="H19" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="J19" s="84"/>
+      <c r="K19" s="85"/>
+      <c r="L19" s="85"/>
+      <c r="M19" s="85"/>
+      <c r="N19" s="86"/>
+    </row>
+    <row r="22" spans="3:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="60" t="s">
         <v>134</v>
       </c>
-      <c r="D19" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="F19" s="58" t="s">
-        <v>126</v>
-      </c>
-      <c r="G19" s="59" t="s">
-        <v>126</v>
-      </c>
-      <c r="H19" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="J19" s="80"/>
-      <c r="K19" s="81"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="81"/>
-      <c r="N19" s="82"/>
-    </row>
-    <row r="22" spans="3:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C22" s="60" t="s">
+      <c r="D22" s="61" t="s">
         <v>135</v>
       </c>
-      <c r="D22" s="61" t="s">
+      <c r="E22" s="62"/>
+      <c r="F22" s="87" t="s">
+        <v>146</v>
+      </c>
+      <c r="G22" s="87"/>
+      <c r="H22" s="87"/>
+      <c r="I22" s="87"/>
+    </row>
+    <row r="23" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C23" s="63" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" s="50" t="s">
+        <v>155</v>
+      </c>
+      <c r="F23" s="81"/>
+      <c r="G23" s="82"/>
+      <c r="H23" s="82"/>
+      <c r="I23" s="83"/>
+    </row>
+    <row r="24" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C24" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="E22" s="62"/>
-      <c r="F22" s="85" t="s">
-        <v>147</v>
-      </c>
-      <c r="G22" s="85"/>
-      <c r="H22" s="85"/>
-      <c r="I22" s="85"/>
-    </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C23" s="63" t="s">
-        <v>146</v>
-      </c>
-      <c r="D23" s="50" t="s">
-        <v>126</v>
-      </c>
-      <c r="F23" s="86"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="88"/>
-    </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C24" s="34" t="s">
-        <v>137</v>
-      </c>
       <c r="D24" s="35" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="F24" s="77"/>
       <c r="G24" s="78"/>
       <c r="H24" s="78"/>
       <c r="I24" s="79"/>
     </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C25" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="D25" s="35"/>
+        <v>144</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>155</v>
+      </c>
       <c r="F25" s="64"/>
       <c r="G25" s="65"/>
       <c r="H25" s="65"/>
       <c r="I25" s="66"/>
     </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C26" s="34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D26" s="35" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="F26" s="77"/>
       <c r="G26" s="78"/>
       <c r="H26" s="78"/>
       <c r="I26" s="79"/>
     </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C27" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="D27" s="35" t="s">
-        <v>126</v>
+        <v>138</v>
+      </c>
+      <c r="D27" s="95" t="s">
+        <v>155</v>
       </c>
       <c r="F27" s="77"/>
       <c r="G27" s="78"/>
       <c r="H27" s="78"/>
       <c r="I27" s="79"/>
     </row>
-    <row r="28" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C28" s="36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D28" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="F28" s="80"/>
-      <c r="G28" s="81"/>
-      <c r="H28" s="81"/>
-      <c r="I28" s="82"/>
+        <v>156</v>
+      </c>
+      <c r="F28" s="84"/>
+      <c r="G28" s="85"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="J17:N17"/>
+    <mergeCell ref="J18:N18"/>
+    <mergeCell ref="J19:N19"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="J12:N12"/>
+    <mergeCell ref="J13:N13"/>
+    <mergeCell ref="J14:N14"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="J16:N16"/>
     <mergeCell ref="J9:N9"/>
     <mergeCell ref="J10:N10"/>
     <mergeCell ref="J11:N11"/>
@@ -2834,22 +2943,8 @@
     <mergeCell ref="J6:N6"/>
     <mergeCell ref="J7:N7"/>
     <mergeCell ref="J8:N8"/>
-    <mergeCell ref="J12:N12"/>
-    <mergeCell ref="J13:N13"/>
-    <mergeCell ref="J14:N14"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="J16:N16"/>
-    <mergeCell ref="J17:N17"/>
-    <mergeCell ref="J18:N18"/>
-    <mergeCell ref="J19:N19"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>